<commit_message>
Arreglos en el informe de recategorizacion
</commit_message>
<xml_diff>
--- a/excel/informe recategorizacion de 2020.0 a EneroJunio.XLSX
+++ b/excel/informe recategorizacion de 2020.0 a EneroJunio.XLSX
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Informe para recategorizacion</t>
   </si>
   <si>
+    <t xml:space="preserve">Montos para la nueva categoria</t>
+  </si>
+  <si>
     <t xml:space="preserve">Detalle</t>
   </si>
   <si>
@@ -38,6 +41,24 @@
   </si>
   <si>
     <t xml:space="preserve">Recategorizacion E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hasta el 30 jun 2020 todavia podes facturar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faltan 3 meses para la proxima recategorizacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por mes podes facturar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuota Mensual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aporte autonomo / Obra social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -154,10 +175,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,25 +193,30 @@
       </c>
       <c r="B1" s="1"/>
     </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>723270.02</v>
+        <v>725070.02</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>834957</v>
@@ -198,10 +224,59 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>834957</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>109886.98</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">+B8/B9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1739.48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>5256.36</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>6995.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>